<commit_message>
Updated data processing pipeline
</commit_message>
<xml_diff>
--- a/data/FHR_Partners_Geocoded.xlsx
+++ b/data/FHR_Partners_Geocoded.xlsx
@@ -633,7 +633,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Kwazulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -669,7 +669,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Kwazulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -688,10 +688,10 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>-29.56871777290991</v>
+        <v>-29.56617368768535</v>
       </c>
       <c r="H7" t="n">
-        <v>30.18431398874813</v>
+        <v>30.18582508164073</v>
       </c>
     </row>
     <row r="8">
@@ -705,7 +705,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Kwazulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>-29.56259963008713</v>
+        <v>-29.56526933488195</v>
       </c>
       <c r="H8" t="n">
-        <v>30.18591236520352</v>
+        <v>30.1768329958818</v>
       </c>
     </row>
     <row r="9">
@@ -760,10 +760,10 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>-23.30751524056666</v>
+        <v>-23.30472086703238</v>
       </c>
       <c r="H9" t="n">
-        <v>30.69405267766082</v>
+        <v>30.70747633816771</v>
       </c>
     </row>
     <row r="10">
@@ -796,10 +796,10 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>-23.30556699485823</v>
+        <v>-23.30549895907519</v>
       </c>
       <c r="H10" t="n">
-        <v>30.70183322839475</v>
+        <v>30.70299779643534</v>
       </c>
     </row>
     <row r="11">
@@ -923,7 +923,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Western Cape </t>
+          <t>Western Cape</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Western Cape </t>
+          <t>Western Cape</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Kwazulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">North West  </t>
+          <t>North West</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Kwazulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Kwazulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Kwazulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">North West  </t>
+          <t>North West</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2160,10 +2160,10 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>-25.67220409677826</v>
+        <v>-25.67561525692701</v>
       </c>
       <c r="I2" t="n">
-        <v>27.235762610813</v>
+        <v>27.23584568333255</v>
       </c>
     </row>
     <row r="3">
@@ -2201,10 +2201,10 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-25.66436619430646</v>
+        <v>-25.67639563630532</v>
       </c>
       <c r="I3" t="n">
-        <v>27.24362815339374</v>
+        <v>27.24686548918428</v>
       </c>
     </row>
     <row r="4">
@@ -2242,10 +2242,10 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>-33.91299762285691</v>
+        <v>-33.91486044871371</v>
       </c>
       <c r="I4" t="n">
-        <v>18.42421966743632</v>
+        <v>18.4303868407082</v>
       </c>
     </row>
     <row r="5">
@@ -2283,10 +2283,10 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-33.91528040018368</v>
+        <v>-33.91843687622078</v>
       </c>
       <c r="I5" t="n">
-        <v>18.41602659327719</v>
+        <v>18.42483316221153</v>
       </c>
     </row>
     <row r="6">
@@ -2324,10 +2324,10 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>-23.84967348799373</v>
+        <v>-23.84121903436854</v>
       </c>
       <c r="I6" t="n">
-        <v>29.37969236241326</v>
+        <v>29.37694249305345</v>
       </c>
     </row>
     <row r="7">
@@ -2365,10 +2365,10 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>-23.84468594628398</v>
+        <v>-23.84114844892832</v>
       </c>
       <c r="I7" t="n">
-        <v>29.37696299168308</v>
+        <v>29.37960026836785</v>
       </c>
     </row>
     <row r="8">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Eastern Cape </t>
+          <t>Eastern Cape</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2406,10 +2406,10 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>-33.91678707369896</v>
+        <v>-33.90650348116984</v>
       </c>
       <c r="I8" t="n">
-        <v>25.58946287834251</v>
+        <v>25.58779022272385</v>
       </c>
     </row>
     <row r="9">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Eastern Cape </t>
+          <t>Eastern Cape</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2447,10 +2447,10 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>-33.905670742895</v>
+        <v>-33.90675649172453</v>
       </c>
       <c r="I9" t="n">
-        <v>25.5852651635365</v>
+        <v>25.58837571349237</v>
       </c>
     </row>
     <row r="10">
@@ -2488,10 +2488,10 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>-30.64115552188461</v>
+        <v>-30.65129098950961</v>
       </c>
       <c r="I10" t="n">
-        <v>24.01793505109065</v>
+        <v>24.01401732006992</v>
       </c>
     </row>
     <row r="11">
@@ -2529,10 +2529,10 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>-30.64959625640029</v>
+        <v>-30.63777962344104</v>
       </c>
       <c r="I11" t="n">
-        <v>24.01196773405263</v>
+        <v>24.00869877999387</v>
       </c>
     </row>
     <row r="12">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>KwaZulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -2570,10 +2570,10 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>-29.60127615536759</v>
+        <v>-29.59647196517574</v>
       </c>
       <c r="I12" t="n">
-        <v>30.38249981693924</v>
+        <v>30.37921417005645</v>
       </c>
     </row>
     <row r="13">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>KwaZulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2611,10 +2611,10 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>-29.60215714107128</v>
+        <v>-29.60054737026591</v>
       </c>
       <c r="I13" t="n">
-        <v>30.376223204914</v>
+        <v>30.37802430166695</v>
       </c>
     </row>
     <row r="14">
@@ -2652,10 +2652,10 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>-29.12792530462544</v>
+        <v>-29.12758616489118</v>
       </c>
       <c r="I14" t="n">
-        <v>26.27676302661703</v>
+        <v>26.28562167835697</v>
       </c>
     </row>
     <row r="15">
@@ -2693,10 +2693,10 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>-29.13710299909996</v>
+        <v>-29.13081182836828</v>
       </c>
       <c r="I15" t="n">
-        <v>26.28289264363866</v>
+        <v>26.28471596254374</v>
       </c>
     </row>
     <row r="16">
@@ -2734,10 +2734,10 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>-29.14091263353026</v>
+        <v>-29.13979741335006</v>
       </c>
       <c r="I16" t="n">
-        <v>26.29188397677818</v>
+        <v>26.28036611426643</v>
       </c>
     </row>
     <row r="17">
@@ -2775,10 +2775,10 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>-29.13539036112939</v>
+        <v>-29.13312496661504</v>
       </c>
       <c r="I17" t="n">
-        <v>26.27843283021459</v>
+        <v>26.28141291430465</v>
       </c>
     </row>
     <row r="18">
@@ -2816,10 +2816,10 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>-26.02111060339211</v>
+        <v>-26.01617497365869</v>
       </c>
       <c r="I18" t="n">
-        <v>28.214922162748</v>
+        <v>28.22529983485829</v>
       </c>
     </row>
     <row r="19">
@@ -2857,10 +2857,10 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>-26.01765650020961</v>
+        <v>-26.00772897785614</v>
       </c>
       <c r="I19" t="n">
-        <v>28.23128058562917</v>
+        <v>28.21686510370403</v>
       </c>
     </row>
     <row r="20">
@@ -2898,10 +2898,10 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>-26.36267765869195</v>
+        <v>-26.35536144556415</v>
       </c>
       <c r="I20" t="n">
-        <v>28.14169796289607</v>
+        <v>28.1443528409034</v>
       </c>
     </row>
     <row r="21">
@@ -2939,10 +2939,10 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>-26.35669655901962</v>
+        <v>-26.36498227083928</v>
       </c>
       <c r="I21" t="n">
-        <v>28.14242286204568</v>
+        <v>28.14407618099457</v>
       </c>
     </row>
     <row r="22">
@@ -2980,10 +2980,10 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>-25.48330638996369</v>
+        <v>-25.47635795003008</v>
       </c>
       <c r="I22" t="n">
-        <v>29.02439490838582</v>
+        <v>29.00746233913173</v>
       </c>
     </row>
     <row r="23">
@@ -3021,10 +3021,10 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>-25.47170254098451</v>
+        <v>-25.4863984750171</v>
       </c>
       <c r="I23" t="n">
-        <v>29.01792508894156</v>
+        <v>29.02125058596489</v>
       </c>
     </row>
     <row r="24">
@@ -3062,10 +3062,10 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>-31.58557040327437</v>
+        <v>-31.59129237924279</v>
       </c>
       <c r="I24" t="n">
-        <v>28.75271600109983</v>
+        <v>28.76622748996408</v>
       </c>
     </row>
     <row r="25">
@@ -3103,10 +3103,10 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>-31.59807337011446</v>
+        <v>-31.59383582131341</v>
       </c>
       <c r="I25" t="n">
-        <v>28.76411475392914</v>
+        <v>28.75713086575806</v>
       </c>
     </row>
     <row r="26">
@@ -3144,10 +3144,10 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>-23.31432047060651</v>
+        <v>-23.30699409606289</v>
       </c>
       <c r="I26" t="n">
-        <v>30.69580108485691</v>
+        <v>30.69488038472128</v>
       </c>
     </row>
     <row r="27">
@@ -3185,10 +3185,10 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>-23.30273277899696</v>
+        <v>-23.31121455460828</v>
       </c>
       <c r="I27" t="n">
-        <v>30.69528336182293</v>
+        <v>30.6948092315841</v>
       </c>
     </row>
     <row r="28">
@@ -3226,10 +3226,10 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>-25.48844732423583</v>
+        <v>-25.48663210322576</v>
       </c>
       <c r="I28" t="n">
-        <v>27.83188206719231</v>
+        <v>27.83662532363554</v>
       </c>
     </row>
     <row r="29">
@@ -3267,10 +3267,10 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>-25.48654253856615</v>
+        <v>-25.48886711686297</v>
       </c>
       <c r="I29" t="n">
-        <v>27.83159275954879</v>
+        <v>27.83626665444433</v>
       </c>
     </row>
     <row r="30">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>KwaZulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>-29.57035230888783</v>
+        <v>-29.55937289129131</v>
       </c>
       <c r="I30" t="n">
-        <v>30.19257725127261</v>
+        <v>30.19448471978172</v>
       </c>
     </row>
     <row r="31">
@@ -3335,7 +3335,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>KwaZulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3349,10 +3349,10 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>-29.57281395092231</v>
+        <v>-29.57737026179612</v>
       </c>
       <c r="I31" t="n">
-        <v>30.17723667931871</v>
+        <v>30.1887879545572</v>
       </c>
     </row>
     <row r="32">
@@ -3390,10 +3390,10 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>-26.03703321996902</v>
+        <v>-26.03136101452483</v>
       </c>
       <c r="I32" t="n">
-        <v>30.7885465997434</v>
+        <v>30.785120257149</v>
       </c>
     </row>
     <row r="33">
@@ -3431,10 +3431,10 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>-26.04360638081151</v>
+        <v>-26.04971293877983</v>
       </c>
       <c r="I33" t="n">
-        <v>30.79967601669371</v>
+        <v>30.79186298832423</v>
       </c>
     </row>
     <row r="34">
@@ -3472,10 +3472,10 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>-24.84367503597136</v>
+        <v>-24.8343291472963</v>
       </c>
       <c r="I34" t="n">
-        <v>31.08150591901412</v>
+        <v>31.07503226936309</v>
       </c>
     </row>
     <row r="35">
@@ -3513,10 +3513,10 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>-24.85087322378515</v>
+        <v>-24.83413127169455</v>
       </c>
       <c r="I35" t="n">
-        <v>31.0718297900195</v>
+        <v>31.07595594527941</v>
       </c>
     </row>
     <row r="36">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Eastern Cape </t>
+          <t>Eastern Cape</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3554,10 +3554,10 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>-31.9124476043067</v>
+        <v>-31.91989986631074</v>
       </c>
       <c r="I36" t="n">
-        <v>26.96407104107173</v>
+        <v>26.96835760417916</v>
       </c>
     </row>
     <row r="37">
@@ -3595,10 +3595,10 @@
         </is>
       </c>
       <c r="H37" t="n">
-        <v>-31.92194825294755</v>
+        <v>-31.92440641570071</v>
       </c>
       <c r="I37" t="n">
-        <v>26.95158125969244</v>
+        <v>26.96170478174716</v>
       </c>
     </row>
     <row r="38">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Eastern Cape </t>
+          <t>Eastern Cape</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3636,10 +3636,10 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>-31.91691198044382</v>
+        <v>-31.91903281002792</v>
       </c>
       <c r="I38" t="n">
-        <v>26.95391516002716</v>
+        <v>26.95859839517394</v>
       </c>
     </row>
     <row r="39">
@@ -3677,10 +3677,10 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>-29.23217551287697</v>
+        <v>-29.22807044592622</v>
       </c>
       <c r="I39" t="n">
-        <v>26.70747221646431</v>
+        <v>26.7137045122598</v>
       </c>
     </row>
     <row r="40">
@@ -3718,10 +3718,10 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>-29.22431783930347</v>
+        <v>-29.23409597626011</v>
       </c>
       <c r="I40" t="n">
-        <v>26.70089526828257</v>
+        <v>26.7050172654635</v>
       </c>
     </row>
     <row r="41">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>-28.74629913524904</v>
+        <v>-28.73917847099753</v>
       </c>
       <c r="I41" t="n">
-        <v>24.75617049102631</v>
+        <v>24.76517568009713</v>
       </c>
     </row>
     <row r="42">
@@ -3800,10 +3800,10 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>-28.74548139994879</v>
+        <v>-28.74098160667427</v>
       </c>
       <c r="I42" t="n">
-        <v>24.77247131058075</v>
+        <v>24.76734260845445</v>
       </c>
     </row>
     <row r="43">
@@ -3841,10 +3841,10 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>-33.92456038111257</v>
+        <v>-33.93523786602753</v>
       </c>
       <c r="I43" t="n">
-        <v>18.86830464493464</v>
+        <v>18.85313351420969</v>
       </c>
     </row>
     <row r="44">
@@ -3882,10 +3882,10 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>-33.92956351645091</v>
+        <v>-33.92743585743257</v>
       </c>
       <c r="I44" t="n">
-        <v>18.86495491497146</v>
+        <v>18.86326339619207</v>
       </c>
     </row>
     <row r="45">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>KwaZulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3923,10 +3923,10 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>-29.56153139920033</v>
+        <v>-29.57466070029357</v>
       </c>
       <c r="I45" t="n">
-        <v>30.17819859701962</v>
+        <v>30.18415094608206</v>
       </c>
     </row>
     <row r="46">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>KwaZulu Natal</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3964,10 +3964,10 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>-29.56977848767361</v>
+        <v>-29.56073443345731</v>
       </c>
       <c r="I46" t="n">
-        <v>30.19332877108758</v>
+        <v>30.17832181777939</v>
       </c>
     </row>
     <row r="47">
@@ -4005,10 +4005,10 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>-23.32176237744271</v>
+        <v>-23.32126218644981</v>
       </c>
       <c r="I47" t="n">
-        <v>30.69358098787117</v>
+        <v>30.70499327015509</v>
       </c>
     </row>
     <row r="48">
@@ -4046,10 +4046,10 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>-23.30386414683187</v>
+        <v>-23.30313154721219</v>
       </c>
       <c r="I48" t="n">
-        <v>30.7077553990093</v>
+        <v>30.70852188236656</v>
       </c>
     </row>
   </sheetData>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">North West </t>
+          <t>North West</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -4440,10 +4440,10 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>-26.19611032137056</v>
+        <v>-26.20779877670934</v>
       </c>
       <c r="I9" t="n">
-        <v>28.03897863450159</v>
+        <v>28.03384461945495</v>
       </c>
     </row>
     <row r="10">
@@ -4563,10 +4563,10 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>-26.20761519579212</v>
+        <v>-26.2021863746939</v>
       </c>
       <c r="I12" t="n">
-        <v>28.02664575056103</v>
+        <v>28.03158767278949</v>
       </c>
     </row>
     <row r="13">
@@ -4604,10 +4604,10 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>-29.85260448094786</v>
+        <v>-29.86424184272459</v>
       </c>
       <c r="I13" t="n">
-        <v>31.0266781834182</v>
+        <v>31.0229213815519</v>
       </c>
     </row>
     <row r="14">
@@ -4645,10 +4645,10 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>-33.92342277157874</v>
+        <v>-33.92560180897983</v>
       </c>
       <c r="I14" t="n">
-        <v>18.41439818203678</v>
+        <v>18.41867477926927</v>
       </c>
     </row>
     <row r="15">
@@ -4686,10 +4686,10 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>-26.19701598060724</v>
+        <v>-26.19961059762062</v>
       </c>
       <c r="I15" t="n">
-        <v>28.0255973930555</v>
+        <v>28.02735632037809</v>
       </c>
     </row>
     <row r="16">
@@ -4809,10 +4809,10 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>-33.95825679555264</v>
+        <v>-33.97358883456565</v>
       </c>
       <c r="I18" t="n">
-        <v>18.50838717757813</v>
+        <v>18.50096177489309</v>
       </c>
     </row>
     <row r="19">
@@ -4850,10 +4850,10 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>-29.85578814721454</v>
+        <v>-29.85373171138816</v>
       </c>
       <c r="I19" t="n">
-        <v>31.03078865566874</v>
+        <v>31.01856758092833</v>
       </c>
     </row>
     <row r="20">
@@ -4891,10 +4891,10 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>-33.91991350184752</v>
+        <v>-33.92638245895357</v>
       </c>
       <c r="I20" t="n">
-        <v>18.42486354465139</v>
+        <v>18.42920592122096</v>
       </c>
     </row>
     <row r="21">
@@ -4932,10 +4932,10 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>-33.97349727585551</v>
+        <v>-33.96541170497592</v>
       </c>
       <c r="I21" t="n">
-        <v>18.50631607544738</v>
+        <v>18.50170394113072</v>
       </c>
     </row>
     <row r="22">
@@ -4973,10 +4973,10 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>-26.20291624192704</v>
+        <v>-26.20219738747916</v>
       </c>
       <c r="I22" t="n">
-        <v>28.03125767117453</v>
+        <v>28.03262283151156</v>
       </c>
     </row>
     <row r="23">
@@ -5055,10 +5055,10 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>-29.85518064658501</v>
+        <v>-29.86484746922991</v>
       </c>
       <c r="I24" t="n">
-        <v>31.02830522362622</v>
+        <v>31.02622780455514</v>
       </c>
     </row>
     <row r="25">

</xml_diff>